<commit_message>
Finished Lab Report 2
</commit_message>
<xml_diff>
--- a/Labs/Lab 2 - Physics of Semiconductors/1 - Two Square Wells - Comparing well separation.xlsx
+++ b/Labs/Lab 2 - Physics of Semiconductors/1 - Two Square Wells - Comparing well separation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Google Drive\University\2018\sem 1\PHYS2170\Labs\Lab 2 - Physics of Semiconductors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\Physics\Physics\Labs\Lab 2 - Physics of Semiconductors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABFD2D3-D006-42A2-96F8-ECE9FB4C6B8F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF82F7B-9C74-493C-BACC-575F532B1987}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" xr2:uid="{51699A8B-FBED-4012-B6B4-ABB827353085}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" xr2:uid="{51699A8B-FBED-4012-B6B4-ABB827353085}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
   <si>
     <t>Single Well</t>
   </si>
@@ -74,12 +74,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -113,36 +130,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Allowed</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> Energies for Two-well Lattice of Varying Separation</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -156,7 +143,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -181,11 +168,8 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>0.0nm Separation</c:v>
-          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -207,40 +191,42 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$31:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$30:$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>Single Well</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>Single Well</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>Single Well</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Single Well</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$31:$B$35</c:f>
+              <c:f>Sheet1!$B$30:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>24.6</c:v>
+                  <c:v>7.59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96.65</c:v>
+                  <c:v>30.28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>208.44</c:v>
+                  <c:v>67.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -248,312 +234,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7D5C-4EEF-A008-B597B495E529}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>0.01nm Separation</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$31:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$31:$C$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>60.96</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>97.88</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>251.71</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7D5C-4EEF-A008-B597B495E529}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>0.05nm Separation</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$31:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$31:$D$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>69.52</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>71.09</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>241.73</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>258.81</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7D5C-4EEF-A008-B597B495E529}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>0.1nm Separation</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$31:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$31:$E$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>70.290000000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>70.31</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>246.92</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>249.1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7D5C-4EEF-A008-B597B495E529}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>Single Well</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$31:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$31:$F$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>7.59</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30.28</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>67.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>119.56</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7D5C-4EEF-A008-B597B495E529}"/>
+              <c16:uniqueId val="{00000000-BC09-4E64-9B2C-F39E23749C7C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -565,15 +246,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="495561616"/>
-        <c:axId val="495562272"/>
+        <c:axId val="621523200"/>
+        <c:axId val="621520248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="495561616"/>
+        <c:axId val="621523200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4"/>
-          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -591,61 +270,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>Principal Quantum Number (n)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
+        <c:numFmt formatCode="@" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621520248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="621520248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -683,18 +369,717 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495562272"/>
+        <c:crossAx val="621523200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Energy Levels of a Two-Well lattice of Varying Separation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>0nm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>208.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D899-4E6C-B63B-787A2685792E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>0.01nm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$19:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>60.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D899-4E6C-B63B-787A2685792E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>0.05nm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$22:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>69.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>241.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>258.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D899-4E6C-B63B-787A2685792E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>0.1nm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$26:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>@</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>70.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>246.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>249.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D899-4E6C-B63B-787A2685792E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="621526808"/>
+        <c:axId val="621523856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="621526808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Well Separation (nm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="@" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621523856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="495562272"/>
+        <c:axId val="621523856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="270"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -702,9 +1087,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -719,11 +1104,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -732,14 +1116,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>Energy</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Energy Level (eV)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" b="1" baseline="0"/>
-                  <a:t> (eV)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -756,11 +1135,10 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -780,12 +1158,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -796,9 +1172,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -809,7 +1184,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495561616"/>
+        <c:crossAx val="621526808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -838,9 +1213,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -864,17 +1238,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -936,6 +1321,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1452,27 +1877,529 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42861</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>109537</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F434272-4A26-4F23-9253-93F0DC4C961C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EC12FB-AED7-4524-ADAC-806A14803982}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1485,6 +2412,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>347661</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6962F614-2472-4A16-9F53-96907A809C3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1790,143 +2753,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E7C17D-4EA8-4D60-809A-3D7D08E7300C}">
-  <dimension ref="A12:F34"/>
+  <dimension ref="A12:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:F34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" style="7" customWidth="1"/>
     <col min="2" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>0</v>
+      </c>
+      <c r="B16" s="5">
+        <v>24.6</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="F16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5">
+        <v>96.65</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>24.6</v>
+      </c>
+      <c r="H17" s="5">
+        <v>96.65</v>
+      </c>
+      <c r="I17" s="5">
+        <v>208.44</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>208.44</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
+      <c r="F18" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G18" s="5">
+        <v>60.96</v>
+      </c>
+      <c r="H18" s="5">
+        <v>97.88</v>
+      </c>
+      <c r="I18" s="5">
+        <v>251.71</v>
+      </c>
+      <c r="J18" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="B19" s="5">
+        <v>60.96</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="F19" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G19" s="5">
+        <v>69.52</v>
+      </c>
+      <c r="H19" s="5">
+        <v>71.09</v>
+      </c>
+      <c r="I19" s="5">
+        <v>241.73</v>
+      </c>
+      <c r="J19" s="5">
+        <v>258.81</v>
+      </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="B20" s="5">
+        <v>97.88</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="F20" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>70.290000000000006</v>
+      </c>
+      <c r="H20" s="5">
+        <v>70.31</v>
+      </c>
+      <c r="I20" s="5">
+        <v>246.92</v>
+      </c>
+      <c r="J20" s="5">
+        <v>249.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="B21" s="5">
+        <v>251.71</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="F21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="G21" s="5">
+        <v>7.59</v>
+      </c>
+      <c r="H21" s="5">
+        <v>30.28</v>
+      </c>
+      <c r="I21" s="5">
+        <v>67.8</v>
+      </c>
+      <c r="J21" s="5">
+        <v>119.56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
         <v>0.05</v>
       </c>
-      <c r="E30" s="2">
+      <c r="B22" s="5">
+        <v>69.52</v>
+      </c>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="B23" s="5">
+        <v>71.09</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="B24" s="5">
+        <v>241.73</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="B25" s="5">
+        <v>258.81</v>
+      </c>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <v>0.1</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="B26" s="5">
+        <v>70.290000000000006</v>
+      </c>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="B27" s="5">
+        <v>70.31</v>
+      </c>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="B28" s="5">
+        <v>246.92</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="B29" s="5">
+        <v>249.1</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="8" t="s">
         <v>0</v>
       </c>
+      <c r="E29" s="5">
+        <v>7.59</v>
+      </c>
+      <c r="F29" s="5">
+        <v>30.28</v>
+      </c>
+      <c r="G29" s="5">
+        <v>67.8</v>
+      </c>
+      <c r="H29" s="5">
+        <v>119.56</v>
+      </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>1</v>
-      </c>
-      <c r="B31">
-        <v>24.6</v>
-      </c>
-      <c r="C31">
-        <v>60.96</v>
-      </c>
-      <c r="D31">
-        <v>69.52</v>
-      </c>
-      <c r="E31">
-        <v>70.290000000000006</v>
-      </c>
-      <c r="F31">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="5">
         <v>7.59</v>
       </c>
+      <c r="C30" s="5"/>
+      <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>2</v>
-      </c>
-      <c r="B32">
-        <v>96.65</v>
-      </c>
-      <c r="C32">
-        <v>97.88</v>
-      </c>
-      <c r="D32">
-        <v>71.09</v>
-      </c>
-      <c r="E32">
-        <v>70.31</v>
-      </c>
-      <c r="F32">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="5">
         <v>30.28</v>
       </c>
+      <c r="C31" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>3</v>
-      </c>
-      <c r="B33">
-        <v>208.44</v>
-      </c>
-      <c r="C33">
-        <v>251.71</v>
-      </c>
-      <c r="D33">
-        <v>241.73</v>
-      </c>
-      <c r="E33">
-        <v>246.92</v>
-      </c>
-      <c r="F33">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="5">
         <v>67.8</v>
       </c>
+      <c r="C32" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>4</v>
-      </c>
-      <c r="D34">
-        <v>258.81</v>
-      </c>
-      <c r="E34">
-        <v>249.1</v>
-      </c>
-      <c r="F34">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="5">
         <v>119.56</v>
       </c>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>